<commit_message>
corrected one species error bovinus and worked further on executive summary
</commit_message>
<xml_diff>
--- a/data/Status_OSPAR_summary.xlsx
+++ b/data/Status_OSPAR_summary.xlsx
@@ -405,14 +405,29 @@
           <t>Gulper shark</t>
         </is>
       </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Not applicable</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Not applicable</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Not applicable</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
@@ -429,7 +444,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Not applicable</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -464,6 +484,11 @@
           <t>Poor</t>
         </is>
       </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Not applicable</t>
+        </is>
+      </c>
       <c r="E4" t="inlineStr">
         <is>
           <t>Poor</t>
@@ -540,17 +565,17 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t xml:space="preserve">? </t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
@@ -567,27 +592,27 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t> ?</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t> ?</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>Unknown</t>
         </is>
       </c>
     </row>
@@ -604,7 +629,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -624,7 +649,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>←→1</t>
+          <t>Stable</t>
         </is>
       </c>
     </row>
@@ -639,6 +664,11 @@
           <t>Spotted ray</t>
         </is>
       </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Not applicable</t>
+        </is>
+      </c>
       <c r="D9" t="inlineStr">
         <is>
           <t>Good</t>
@@ -646,12 +676,17 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Not applicable</t>
         </is>
       </c>
     </row>
@@ -666,6 +701,11 @@
           <t>White skate</t>
         </is>
       </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Not applicable</t>
+        </is>
+      </c>
       <c r="D10" t="inlineStr">
         <is>
           <t>Poor</t>
@@ -679,6 +719,11 @@
       <c r="F10" t="inlineStr">
         <is>
           <t>Poor</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Not applicable</t>
         </is>
       </c>
     </row>
@@ -693,6 +738,11 @@
           <t>Angelshark</t>
         </is>
       </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Not applicable</t>
+        </is>
+      </c>
       <c r="D11" t="inlineStr">
         <is>
           <t>Poor</t>
@@ -700,12 +750,17 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Poor2</t>
+          <t>Poor</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
           <t>Poor</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Not applicable</t>
         </is>
       </c>
     </row>

</xml_diff>